<commit_message>
updated newMain, added sql file to create db
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="N34" sqref="N33:N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated newMain to include SQL export, added test files
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/846f05906f3c79a7/Documents/isbn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{387E5A72-074B-8A41-8DC8-E91BF738376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E95662A0-0266-4036-A905-148422948AC8}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{387E5A72-074B-8A41-8DC8-E91BF738376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD5D0625-E864-4C2A-9A77-40466CF2A164}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>isbn's</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>last retutned record line 26 9781838981778</t>
+  </si>
+  <si>
+    <t>genre</t>
   </si>
 </sst>
 </file>
@@ -415,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N34" sqref="N33:N34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,30 +432,48 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>9780073517216</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>9780201563177</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>9781593272203</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>9780764548338</v>
       </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9781565924277</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
       </c>
       <c r="K6" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
add more test files, updated newMain to include list preprocessing and db exporting
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/846f05906f3c79a7/Documents/isbn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{387E5A72-074B-8A41-8DC8-E91BF738376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD5D0625-E864-4C2A-9A77-40466CF2A164}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{387E5A72-074B-8A41-8DC8-E91BF738376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DBE5F89-7F9D-4FD1-8119-C6FF54179CA6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>isbn's</t>
-  </si>
-  <si>
     <t>removed at 9 9780471164838</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>genre</t>
+  </si>
+  <si>
+    <t>isbn</t>
   </si>
 </sst>
 </file>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +430,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -448,13 +448,10 @@
       <c r="A3" s="1">
         <v>9780201563177</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>9781593272203</v>
+        <v>9780201563177</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -462,314 +459,322 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>9780764548338</v>
+        <v>9781593272203</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>9781565924277</v>
+        <v>9780764548338</v>
       </c>
       <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>9780471168942</v>
+        <v>9781565924277</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>9780672311079</v>
+        <v>9780471168942</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>9781491931257</v>
+        <v>9780672311079</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9781491979808</v>
+        <v>9781491931257</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9781491924358</v>
-      </c>
-      <c r="N11" s="3">
-        <v>27</v>
+        <v>9781491979808</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>9781449387860</v>
+        <v>9781491924358</v>
+      </c>
+      <c r="N12" s="3">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>9781578700479</v>
+        <v>9781449387860</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>9780132360395</v>
+        <v>9781578700479</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>9780596000257</v>
+        <v>9780132360395</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>9781593273897</v>
+        <v>9780596000257</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>9780134496009</v>
+        <v>9781593273897</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>9781118983843</v>
+        <v>9780134496009</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>9781119722335</v>
+        <v>9781118983843</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>9780134277554</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>2</v>
+        <v>9781119722335</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>9780130206015</v>
+        <v>9780134277554</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>9781509300914</v>
+        <v>9780130206015</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>9781788990554</v>
+        <v>9781509300914</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>9781784399597</v>
+        <v>9781788990554</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>9781800564640</v>
+        <v>9781784399597</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
+        <v>9781800564640</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>9781838981778</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>9781703404609</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>9780471946939</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>9780982131428</v>
+        <v>9780471946939</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>9781617294167</v>
+        <v>9780982131428</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>9781617295096</v>
+        <v>9781617294167</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>9781593279189</v>
+        <v>9781617295096</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>9781565924956</v>
+        <v>9781593279189</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>9780596000035</v>
+        <v>9781565924956</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>9781565927094</v>
+        <v>9780596000035</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>9781491927571</v>
+        <v>9781565927094</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>9781449305352</v>
+        <v>9781491927571</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>9781784390891</v>
+        <v>9781449305352</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>9781492057697</v>
+        <v>9781784390891</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>9781430218333</v>
+        <v>9781492057697</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>9781449316389</v>
+        <v>9781430218333</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>9781119572671</v>
+        <v>9781449316389</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>9781839214189</v>
+        <v>9781119572671</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>9781617293726</v>
+        <v>9781839214189</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>9781838820756</v>
+        <v>9781617293726</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>9781838983444</v>
+        <v>9781838820756</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>9781617296987</v>
+        <v>9781838983444</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>9781491929124</v>
+        <v>9781617296987</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>9781492040767</v>
+        <v>9781491929124</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>9781838552183</v>
+        <v>9781492040767</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>9781484269206</v>
+        <v>9781838552183</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>9798653385322</v>
+        <v>9781484269206</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>9781617294440</v>
+        <v>9798653385322</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>9781617297625</v>
+        <v>9781617294440</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>9781305880290</v>
+        <v>9781617297625</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>9780789735973</v>
+        <v>9781305880290</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>9780072263503</v>
+        <v>9780789735973</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>9781617297519</v>
+        <v>9780072263503</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>9781617295508</v>
+        <v>9781617297519</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>9781617295980</v>
+        <v>9781617295508</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>9780134000022</v>
+        <v>9781617295980</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>9780201835953</v>
+        <v>9780134000022</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
+        <v>9780201835953</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>9781449357016</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added documentation and comments to newMain
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="56" documentId="8_{387E5A72-074B-8A41-8DC8-E91BF738376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DBE5F89-7F9D-4FD1-8119-C6FF54179CA6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="1290" windowWidth="22485" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added genre import to newMain
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/846f05906f3c79a7/Documents/isbn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{387E5A72-074B-8A41-8DC8-E91BF738376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DBE5F89-7F9D-4FD1-8119-C6FF54179CA6}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{387E5A72-074B-8A41-8DC8-E91BF738376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BEEA89B-8F8D-4FF2-8CDE-55643E886C7B}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="1290" windowWidth="22485" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1290" windowWidth="22485" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -418,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,10 +489,16 @@
       <c r="A8" s="1">
         <v>9780471168942</v>
       </c>
+      <c r="B8">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>9780672311079</v>
+      </c>
+      <c r="B9">
+        <v>555</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added complete progran fucntions menu and actions
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="84" documentId="8_{387E5A72-074B-8A41-8DC8-E91BF738376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAB346B2-5B0B-4DF1-8C32-676A1350C7BF}"/>
   <bookViews>
-    <workbookView xWindow="50880" yWindow="3570" windowWidth="22485" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1290" windowWidth="22485" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>